<commit_message>
fixed spelling error on main
</commit_message>
<xml_diff>
--- a/Tables and graphs.xlsx
+++ b/Tables and graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leono\Documents\DAProject2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D9835A-B2D1-47D0-98E0-3407DC85D147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DBC17F-3081-421C-A63F-DA5568C0A496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{1DCB4A85-12B3-4571-8B11-7F6E8D513B34}"/>
   </bookViews>
@@ -1360,6 +1360,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>ILP Algorithm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4058,16 +4083,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>509587</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5032,7 +5057,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>